<commit_message>
Updated the python script to be more scalable
</commit_message>
<xml_diff>
--- a/Utilities/game_titles.xlsx
+++ b/Utilities/game_titles.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UpdateTitlesJson\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UpdateTitlesJson\NEW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7846EB29-ECA7-4630-A6B8-1DFE33D52A43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F089800-84EA-4EAC-8D59-67269C5C440E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alphabet" sheetId="1" r:id="rId1"/>
     <sheet name="grammar" sheetId="2" r:id="rId2"/>
     <sheet name="shapes" sheetId="3" r:id="rId3"/>
     <sheet name="writing" sheetId="4" r:id="rId4"/>
+    <sheet name="Pehla School" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="221">
   <si>
     <t>name</t>
   </si>
@@ -630,16 +631,67 @@
     <t>Cake Layer</t>
   </si>
   <si>
-    <t>बादलों में उड़ो</t>
-  </si>
-  <si>
-    <t>सब्जी मंडी</t>
-  </si>
-  <si>
     <t>पिज़्ज़ा बनाओ</t>
   </si>
   <si>
     <t>आइसक्रीम गिराओ</t>
+  </si>
+  <si>
+    <t>सब्ज़ी मंडी</t>
+  </si>
+  <si>
+    <t>बादलों मै उड़ो</t>
+  </si>
+  <si>
+    <t>en_name</t>
+  </si>
+  <si>
+    <t>hi_name</t>
+  </si>
+  <si>
+    <t>Moving Insects</t>
+  </si>
+  <si>
+    <t>कीड़े की गिनती</t>
+  </si>
+  <si>
+    <t>Insect Counting</t>
+  </si>
+  <si>
+    <t>Multiplication Lamp</t>
+  </si>
+  <si>
+    <t>गुणा पट्ट</t>
+  </si>
+  <si>
+    <t>गुणा बल्ब</t>
+  </si>
+  <si>
+    <t>Math Kicker</t>
+  </si>
+  <si>
+    <t>मैथ्स किकर</t>
+  </si>
+  <si>
+    <t>मैथ किकर</t>
+  </si>
+  <si>
+    <t>Book with Quiz</t>
+  </si>
+  <si>
+    <t>प्रश्नोत्तरी के साथ बुक करें</t>
+  </si>
+  <si>
+    <t>प्रश्नोत्तरी की किताब</t>
+  </si>
+  <si>
+    <t>Book Quiz</t>
+  </si>
+  <si>
+    <t>new_hi_name</t>
+  </si>
+  <si>
+    <t>new_eng_name</t>
   </si>
 </sst>
 </file>
@@ -675,8 +727,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1224,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,7 +1439,7 @@
         <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1469,7 +1522,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,8 +1719,8 @@
       <c r="C15" t="s">
         <v>135</v>
       </c>
-      <c r="D15" t="s">
-        <v>201</v>
+      <c r="D15" s="1" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1681,7 +1734,7 @@
         <v>138</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1737,7 +1790,7 @@
         <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1769,11 +1822,8 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D15" r:id="rId1" display="https://khabar.ndtv.com/topic/%E0%A4%B8%E0%A4%AC%E0%A5%8D%E0%A4%9C%E0%A5%80-%E0%A4%AE%E0%A4%82%E0%A4%A1%E0%A5%80" xr:uid="{DB0085B9-B27E-425D-828F-F8F2D97BFA80}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1874,4 +1924,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C52E422-BD19-4A2B-8D40-706E032D587A}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>